<commit_message>
chore(xlsx): saved files as xslx again
</commit_message>
<xml_diff>
--- a/R/data/dictionaries/1_0/1_0_monthly_repeated.xlsx
+++ b/R/data/dictionaries/1_0/1_0_monthly_repeated.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10909"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9191d99891275c14/Documents/Angela/LifeCycle/Manual/WP1  package/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sido/RProjects/analysis-protocols/R/data/dictionaries/1_0/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9419732F-4CA1-4480-AF71-8A83103AE84D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{0BFB0AE1-4B6B-4E4A-AA6A-163CA6BD48C3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Variables" sheetId="1" r:id="rId1"/>
@@ -713,16 +713,16 @@
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.81640625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="15.453125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="14.453125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="42.453125" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="8.81640625" style="1"/>
+    <col min="1" max="1" width="15.83203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="15.5" style="1" customWidth="1"/>
+    <col min="3" max="3" width="14.5" style="1" customWidth="1"/>
+    <col min="4" max="4" width="42.5" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -791,7 +791,7 @@
       <c r="BF1"/>
       <c r="BG1"/>
     </row>
-    <row r="2" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>30</v>
       </c>
@@ -860,7 +860,7 @@
       <c r="BF2"/>
       <c r="BG2"/>
     </row>
-    <row r="3" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
@@ -875,7 +875,7 @@
       </c>
       <c r="E3"/>
     </row>
-    <row r="4" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>36</v>
       </c>
@@ -890,7 +890,7 @@
       </c>
       <c r="E4"/>
     </row>
-    <row r="5" spans="1:59" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:59" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>31</v>
       </c>
@@ -904,7 +904,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="6" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>32</v>
       </c>
@@ -919,7 +919,7 @@
       </c>
       <c r="E6"/>
     </row>
-    <row r="7" spans="1:59" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:59" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
         <v>33</v>
       </c>
@@ -933,7 +933,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="8" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
         <v>34</v>
       </c>
@@ -947,7 +947,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="9" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="7" t="s">
         <v>35</v>
       </c>
@@ -978,13 +978,13 @@
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.81640625" style="1" customWidth="1"/>
-    <col min="2" max="16384" width="8.81640625" style="1"/>
+    <col min="1" max="1" width="12.83203125" style="1" customWidth="1"/>
+    <col min="2" max="16384" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>11</v>
       </c>
@@ -998,7 +998,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -1012,7 +1012,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
@@ -1026,7 +1026,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
@@ -1040,7 +1040,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>6</v>
       </c>
@@ -1054,7 +1054,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>6</v>
       </c>
@@ -1068,7 +1068,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>6</v>
       </c>
@@ -1082,7 +1082,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>6</v>
       </c>
@@ -1096,7 +1096,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>6</v>
       </c>
@@ -1110,7 +1110,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>6</v>
       </c>
@@ -1124,7 +1124,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>6</v>
       </c>
@@ -1138,7 +1138,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>6</v>
       </c>
@@ -1152,7 +1152,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>6</v>
       </c>
@@ -1166,7 +1166,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>6</v>
       </c>
@@ -1180,7 +1180,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>6</v>
       </c>
@@ -1194,7 +1194,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
         <v>6</v>
       </c>
@@ -1208,7 +1208,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
         <v>6</v>
       </c>
@@ -1222,7 +1222,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
         <v>6</v>
       </c>
@@ -1236,7 +1236,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
         <v>6</v>
       </c>
@@ -1250,7 +1250,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
         <v>6</v>
       </c>

</xml_diff>

<commit_message>
fix(missing): updated missing values in data dicts
</commit_message>
<xml_diff>
--- a/R/data/dictionaries/1_0/1_0_monthly_repeated.xlsx
+++ b/R/data/dictionaries/1_0/1_0_monthly_repeated.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sido/RProjects/analysis-protocols/R/data/dictionaries/1_0/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0BFB0AE1-4B6B-4E4A-AA6A-163CA6BD48C3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC6E5192-582C-6744-8B5B-E2E8AFB41C99}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Variables" sheetId="1" r:id="rId1"/>
@@ -709,7 +709,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BG9"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
@@ -974,8 +974,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3:C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1005,7 +1005,7 @@
       <c r="B2" s="3">
         <v>101</v>
       </c>
-      <c r="C2" s="5">
+      <c r="C2" s="5" t="b">
         <v>0</v>
       </c>
       <c r="D2" s="2" t="s">
@@ -1019,7 +1019,7 @@
       <c r="B3" s="3">
         <v>102</v>
       </c>
-      <c r="C3" s="5">
+      <c r="C3" s="5" t="b">
         <v>0</v>
       </c>
       <c r="D3" s="2" t="s">
@@ -1033,7 +1033,7 @@
       <c r="B4" s="3">
         <v>103</v>
       </c>
-      <c r="C4" s="5">
+      <c r="C4" s="5" t="b">
         <v>0</v>
       </c>
       <c r="D4" s="2" t="s">
@@ -1047,7 +1047,7 @@
       <c r="B5" s="3">
         <v>104</v>
       </c>
-      <c r="C5" s="5">
+      <c r="C5" s="5" t="b">
         <v>0</v>
       </c>
       <c r="D5" s="2" t="s">
@@ -1061,7 +1061,7 @@
       <c r="B6" s="3">
         <v>105</v>
       </c>
-      <c r="C6" s="5">
+      <c r="C6" s="5" t="b">
         <v>0</v>
       </c>
       <c r="D6" s="2" t="s">
@@ -1075,7 +1075,7 @@
       <c r="B7" s="3">
         <v>106</v>
       </c>
-      <c r="C7" s="5">
+      <c r="C7" s="5" t="b">
         <v>0</v>
       </c>
       <c r="D7" s="2" t="s">
@@ -1089,7 +1089,7 @@
       <c r="B8" s="3">
         <v>107</v>
       </c>
-      <c r="C8" s="5">
+      <c r="C8" s="5" t="b">
         <v>0</v>
       </c>
       <c r="D8" s="2" t="s">
@@ -1103,7 +1103,7 @@
       <c r="B9" s="3">
         <v>108</v>
       </c>
-      <c r="C9" s="5">
+      <c r="C9" s="5" t="b">
         <v>0</v>
       </c>
       <c r="D9" s="2" t="s">
@@ -1117,7 +1117,7 @@
       <c r="B10" s="3">
         <v>109</v>
       </c>
-      <c r="C10" s="5">
+      <c r="C10" s="5" t="b">
         <v>0</v>
       </c>
       <c r="D10" s="2" t="s">
@@ -1131,7 +1131,7 @@
       <c r="B11" s="3">
         <v>110</v>
       </c>
-      <c r="C11" s="5">
+      <c r="C11" s="5" t="b">
         <v>0</v>
       </c>
       <c r="D11" s="2" t="s">
@@ -1145,7 +1145,7 @@
       <c r="B12" s="3">
         <v>111</v>
       </c>
-      <c r="C12" s="5">
+      <c r="C12" s="5" t="b">
         <v>0</v>
       </c>
       <c r="D12" s="2" t="s">
@@ -1159,7 +1159,7 @@
       <c r="B13" s="3">
         <v>112</v>
       </c>
-      <c r="C13" s="5">
+      <c r="C13" s="5" t="b">
         <v>0</v>
       </c>
       <c r="D13" s="2" t="s">
@@ -1173,7 +1173,7 @@
       <c r="B14" s="3">
         <v>113</v>
       </c>
-      <c r="C14" s="5">
+      <c r="C14" s="5" t="b">
         <v>0</v>
       </c>
       <c r="D14" s="2" t="s">
@@ -1187,7 +1187,7 @@
       <c r="B15" s="3">
         <v>114</v>
       </c>
-      <c r="C15" s="5">
+      <c r="C15" s="5" t="b">
         <v>0</v>
       </c>
       <c r="D15" s="2" t="s">
@@ -1201,7 +1201,7 @@
       <c r="B16" s="3">
         <v>115</v>
       </c>
-      <c r="C16" s="5">
+      <c r="C16" s="5" t="b">
         <v>0</v>
       </c>
       <c r="D16" s="2" t="s">
@@ -1215,7 +1215,7 @@
       <c r="B17" s="3">
         <v>116</v>
       </c>
-      <c r="C17" s="5">
+      <c r="C17" s="5" t="b">
         <v>0</v>
       </c>
       <c r="D17" s="2" t="s">
@@ -1229,7 +1229,7 @@
       <c r="B18" s="3">
         <v>117</v>
       </c>
-      <c r="C18" s="5">
+      <c r="C18" s="5" t="b">
         <v>0</v>
       </c>
       <c r="D18" s="2" t="s">
@@ -1243,7 +1243,7 @@
       <c r="B19" s="3">
         <v>118</v>
       </c>
-      <c r="C19" s="5">
+      <c r="C19" s="5" t="b">
         <v>0</v>
       </c>
       <c r="D19" s="4" t="s">
@@ -1257,7 +1257,7 @@
       <c r="B20" s="3">
         <v>119</v>
       </c>
-      <c r="C20" s="5">
+      <c r="C20" s="5" t="b">
         <v>0</v>
       </c>
       <c r="D20" s="4" t="s">

</xml_diff>

<commit_message>
chore(cat-cleanup): cleaned up the categories
</commit_message>
<xml_diff>
--- a/R/data/dictionaries/1_0/1_0_monthly_repeated.xlsx
+++ b/R/data/dictionaries/1_0/1_0_monthly_repeated.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sido/RProjects/analysis-protocols/R/data/dictionaries/1_0/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC6E5192-582C-6744-8B5B-E2E8AFB41C99}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09F9DB15-E060-474B-BB59-07F521D77D14}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Variables" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="28">
   <si>
     <t>name</t>
   </si>
@@ -41,9 +41,6 @@
     <t>numeric</t>
   </si>
   <si>
-    <t>cohort_id</t>
-  </si>
-  <si>
     <t>decimal</t>
   </si>
   <si>
@@ -62,57 +59,6 @@
     <t>missing</t>
   </si>
   <si>
-    <t>Gen R</t>
-  </si>
-  <si>
-    <t>INMA</t>
-  </si>
-  <si>
-    <t>NINFEA</t>
-  </si>
-  <si>
-    <t>SWS</t>
-  </si>
-  <si>
-    <t>ALSPAC</t>
-  </si>
-  <si>
-    <t>DNBC</t>
-  </si>
-  <si>
-    <t>BIB</t>
-  </si>
-  <si>
-    <t>GECKO</t>
-  </si>
-  <si>
-    <t>RHEA</t>
-  </si>
-  <si>
-    <t>MOBA</t>
-  </si>
-  <si>
-    <t>ELFE</t>
-  </si>
-  <si>
-    <t>EDEN</t>
-  </si>
-  <si>
-    <t>NFBC66</t>
-  </si>
-  <si>
-    <t>NFBC86</t>
-  </si>
-  <si>
-    <t>HBCS</t>
-  </si>
-  <si>
-    <t>CHOP</t>
-  </si>
-  <si>
-    <t>RAINE</t>
-  </si>
-  <si>
     <t>row_id</t>
   </si>
   <si>
@@ -132,12 +78,6 @@
   </si>
   <si>
     <t>age_years</t>
-  </si>
-  <si>
-    <t>RUG1</t>
-  </si>
-  <si>
-    <t>RUG2</t>
   </si>
   <si>
     <t>label</t>
@@ -235,13 +175,11 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
@@ -710,7 +648,7 @@
   <dimension ref="A1:BG9"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -723,7 +661,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
@@ -733,7 +671,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>39</v>
+        <v>19</v>
       </c>
       <c r="E1"/>
       <c r="F1"/>
@@ -792,8 +730,8 @@
       <c r="BG1"/>
     </row>
     <row r="2" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="4" t="s">
-        <v>30</v>
+      <c r="A2" s="3" t="s">
+        <v>12</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>4</v>
@@ -802,7 +740,7 @@
         <v>5</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="E2"/>
       <c r="F2"/>
@@ -871,13 +809,13 @@
         <v>5</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>41</v>
+        <v>21</v>
       </c>
       <c r="E3"/>
     </row>
     <row r="4" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>36</v>
+        <v>18</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>4</v>
@@ -886,13 +824,13 @@
         <v>5</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>42</v>
+        <v>22</v>
       </c>
       <c r="E4"/>
     </row>
     <row r="5" spans="1:59" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>31</v>
+        <v>13</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>4</v>
@@ -901,64 +839,64 @@
         <v>5</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>43</v>
+        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>44</v>
+      <c r="A6" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>24</v>
       </c>
       <c r="E6"/>
     </row>
     <row r="7" spans="1:59" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="B7" s="7" t="s">
+      <c r="A7" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>45</v>
+      <c r="C7" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="8" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>46</v>
+      <c r="A8" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="B9" s="7" t="s">
+      <c r="A9" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C9" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="D9" s="6" t="s">
-        <v>47</v>
+      <c r="C9" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -972,10 +910,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:D20"/>
+  <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3:C20"/>
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -986,282 +924,16 @@
   <sheetData>
     <row r="1" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" s="3">
-        <v>101</v>
-      </c>
-      <c r="C2" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="3">
-        <v>102</v>
-      </c>
-      <c r="C3" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="3">
-        <v>103</v>
-      </c>
-      <c r="C4" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="3">
-        <v>104</v>
-      </c>
-      <c r="C5" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" s="3">
-        <v>105</v>
-      </c>
-      <c r="C6" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" s="3">
-        <v>106</v>
-      </c>
-      <c r="C7" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8" s="3">
-        <v>107</v>
-      </c>
-      <c r="C8" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="D8" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>19</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B9" s="3">
-        <v>108</v>
-      </c>
-      <c r="C9" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B10" s="3">
-        <v>109</v>
-      </c>
-      <c r="C10" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B11" s="3">
-        <v>110</v>
-      </c>
-      <c r="C11" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B12" s="3">
-        <v>111</v>
-      </c>
-      <c r="C12" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B13" s="3">
-        <v>112</v>
-      </c>
-      <c r="C13" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B14" s="3">
-        <v>113</v>
-      </c>
-      <c r="C14" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B15" s="3">
-        <v>114</v>
-      </c>
-      <c r="C15" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B16" s="3">
-        <v>115</v>
-      </c>
-      <c r="C16" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B17" s="3">
-        <v>116</v>
-      </c>
-      <c r="C17" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B18" s="3">
-        <v>117</v>
-      </c>
-      <c r="C18" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B19" s="3">
-        <v>118</v>
-      </c>
-      <c r="C19" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="D19" s="4" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B20" s="3">
-        <v>119</v>
-      </c>
-      <c r="C20" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="D20" s="4" t="s">
-        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix(monthly): added missing values
</commit_message>
<xml_diff>
--- a/R/data/dictionaries/1_0/1_0_monthly_repeated.xlsx
+++ b/R/data/dictionaries/1_0/1_0_monthly_repeated.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sido/RProjects/analysis-protocols/R/data/dictionaries/1_0/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09F9DB15-E060-474B-BB59-07F521D77D14}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E8966B4-C8C5-8546-A31B-746070285391}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="29">
   <si>
     <t>name</t>
   </si>
@@ -56,9 +56,6 @@
     <t>variable</t>
   </si>
   <si>
-    <t>missing</t>
-  </si>
-  <si>
     <t>row_id</t>
   </si>
   <si>
@@ -105,6 +102,12 @@
   </si>
   <si>
     <t>Age of the child at weight measurement</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>isMissing</t>
   </si>
 </sst>
 </file>
@@ -648,7 +651,7 @@
   <dimension ref="A1:BG9"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="A5" sqref="A5:A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -671,7 +674,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E1"/>
       <c r="F1"/>
@@ -731,7 +734,7 @@
     </row>
     <row r="2" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>4</v>
@@ -740,7 +743,7 @@
         <v>5</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E2"/>
       <c r="F2"/>
@@ -809,13 +812,13 @@
         <v>5</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E3"/>
     </row>
     <row r="4" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>4</v>
@@ -824,13 +827,13 @@
         <v>5</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E4"/>
     </row>
     <row r="5" spans="1:59" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>4</v>
@@ -839,12 +842,12 @@
         <v>5</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>6</v>
@@ -853,13 +856,13 @@
         <v>8</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E6"/>
     </row>
     <row r="7" spans="1:59" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B7" s="5" t="s">
         <v>4</v>
@@ -868,12 +871,12 @@
         <v>7</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="8" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>6</v>
@@ -882,12 +885,12 @@
         <v>9</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="9" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B9" s="5" t="s">
         <v>4</v>
@@ -896,7 +899,7 @@
         <v>7</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -910,10 +913,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -930,10 +933,94 @@
         <v>0</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>11</v>
+        <v>28</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C5" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix(cat-missing): fix the missing values evalaute them to an empty space
</commit_message>
<xml_diff>
--- a/R/data/dictionaries/1_0/1_0_monthly_repeated.xlsx
+++ b/R/data/dictionaries/1_0/1_0_monthly_repeated.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sido/RProjects/analysis-protocols/R/data/dictionaries/1_0/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sido/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E8966B4-C8C5-8546-A31B-746070285391}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39116509-7AE4-6848-943F-E4D9ACA42D19}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Variables" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="28">
   <si>
     <t>name</t>
   </si>
@@ -102,9 +102,6 @@
   </si>
   <si>
     <t>Age of the child at weight measurement</t>
-  </si>
-  <si>
-    <t>NA</t>
   </si>
   <si>
     <t>isMissing</t>
@@ -651,7 +648,7 @@
   <dimension ref="A1:BG9"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:A9"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -913,10 +910,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="A2" sqref="A2:XFD20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -933,94 +930,10 @@
         <v>0</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>18</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C2" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C3" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C4" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C5" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C6" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C7" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix(row_id): added row_id to non_repeated measures
</commit_message>
<xml_diff>
--- a/R/data/dictionaries/1_0/1_0_monthly_repeated.xlsx
+++ b/R/data/dictionaries/1_0/1_0_monthly_repeated.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sido/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sido/RProjects/analysis-protocols/R/data/dictionaries/1_0/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39116509-7AE4-6848-943F-E4D9ACA42D19}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3658223B-DE1F-2A46-9B58-D84AF4785288}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Variables" sheetId="1" r:id="rId1"/>
@@ -80,9 +80,6 @@
     <t>label</t>
   </si>
   <si>
-    <t>Unique identifier for the row</t>
-  </si>
-  <si>
     <t>Unique identifier for the child</t>
   </si>
   <si>
@@ -105,6 +102,9 @@
   </si>
   <si>
     <t>isMissing</t>
+  </si>
+  <si>
+    <t>Unique identifier for the row in Opal</t>
   </si>
 </sst>
 </file>
@@ -647,8 +647,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BG9"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -740,7 +740,7 @@
         <v>5</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="E2"/>
       <c r="F2"/>
@@ -809,7 +809,7 @@
         <v>5</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E3"/>
     </row>
@@ -824,7 +824,7 @@
         <v>5</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E4"/>
     </row>
@@ -839,7 +839,7 @@
         <v>5</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -853,7 +853,7 @@
         <v>8</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E6"/>
     </row>
@@ -868,7 +868,7 @@
         <v>7</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="8" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -882,7 +882,7 @@
         <v>9</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -896,7 +896,7 @@
         <v>7</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -912,8 +912,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D1"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD20"/>
+    <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -930,7 +930,7 @@
         <v>0</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>18</v>

</xml_diff>